<commit_message>
Bugfixes and threaded loading
</commit_message>
<xml_diff>
--- a/Documentation/Experiment Results.xlsx
+++ b/Documentation/Experiment Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\David\Documents\Work\University\Year 4\Honours\Honours-Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F64ED6-233E-495E-8701-5D1C403A21CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA5AB4C-D46A-4CC1-8C32-DCDE629803CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{C7F0B173-7606-40FF-A663-42595F1E1281}"/>
   </bookViews>
@@ -7563,7 +7563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF49AB30-77D7-4961-9F78-8186E42E6165}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -7729,7 +7729,7 @@
         <v>92.68</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D12" si="1">AVERAGE(B9:C9)</f>
+        <f t="shared" ref="D9" si="1">AVERAGE(B9:C9)</f>
         <v>94.675000000000011</v>
       </c>
       <c r="E9">

</xml_diff>